<commit_message>
Sauvegarde avant intégration composant nav à racine (renommage shop --> app etc.)
</commit_message>
<xml_diff>
--- a/assets/Données/Product.xlsx
+++ b/assets/Données/Product.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/maison-marey/assets/Données/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091E4E42-A80A-5E49-BC27-76A6175074FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203124F6-A0F7-0D42-B317-59E30C9F3D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{A8607C82-8C2C-9441-9D5B-6B1751B24D1C}"/>
   </bookViews>
@@ -751,7 +751,7 @@
   <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>